<commit_message>
more notebooks and csv
</commit_message>
<xml_diff>
--- a/StockAIClean3.xlsx
+++ b/StockAIClean3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soobi\Desktop\Data Bootcamp\source\final-group-project-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F66AA789-8C35-4CA8-9968-9332EB645E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7479E13-CA9D-4EE9-82C3-7FC61B48E6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StockAIClean3" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="193">
   <si>
     <t>No.</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Mid Cap</t>
-  </si>
-  <si>
-    <t>Sm</t>
   </si>
   <si>
     <t>Hold</t>
@@ -10623,10 +10620,10 @@
   <dimension ref="A1:W73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B84" sqref="B84"/>
+      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10707,10 +10704,10 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U1" t="s">
         <v>18</v>
@@ -10719,7 +10716,7 @@
         <v>19</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -11060,13 +11057,13 @@
         <v>29</v>
       </c>
       <c r="Q6" t="s">
+        <v>60</v>
+      </c>
+      <c r="R6" t="s">
         <v>44</v>
       </c>
-      <c r="R6" t="s">
-        <v>45</v>
-      </c>
       <c r="S6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T6" t="s">
         <v>24</v>
@@ -11087,10 +11084,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -11138,7 +11135,7 @@
         <v>30</v>
       </c>
       <c r="S7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
@@ -11159,10 +11156,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -11231,13 +11228,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
@@ -11303,10 +11300,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -11348,7 +11345,7 @@
         <v>29</v>
       </c>
       <c r="Q10" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R10" t="s">
         <v>30</v>
@@ -11375,10 +11372,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -11426,7 +11423,7 @@
         <v>30</v>
       </c>
       <c r="S11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T11" t="s">
         <v>24</v>
@@ -11447,10 +11444,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
         <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -11519,10 +11516,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -11531,7 +11528,7 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
@@ -11564,13 +11561,13 @@
         <v>29</v>
       </c>
       <c r="Q13" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R13" t="s">
         <v>30</v>
       </c>
       <c r="S13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T13" t="s">
         <v>24</v>
@@ -11591,10 +11588,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -11663,13 +11660,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -11714,7 +11711,7 @@
         <v>30</v>
       </c>
       <c r="S15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T15" t="s">
         <v>24</v>
@@ -11735,13 +11732,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -11807,19 +11804,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
         <v>69</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
@@ -11852,13 +11849,13 @@
         <v>40</v>
       </c>
       <c r="Q17" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R17" t="s">
         <v>30</v>
       </c>
       <c r="S17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T17" t="s">
         <v>26</v>
@@ -11879,13 +11876,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
@@ -11930,7 +11927,7 @@
         <v>30</v>
       </c>
       <c r="S18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T18" t="s">
         <v>26</v>
@@ -11951,19 +11948,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>77</v>
       </c>
-      <c r="E19" t="s">
-        <v>78</v>
-      </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>25</v>
@@ -11996,13 +11993,13 @@
         <v>29</v>
       </c>
       <c r="Q19" t="s">
+        <v>60</v>
+      </c>
+      <c r="R19" t="s">
         <v>44</v>
       </c>
-      <c r="R19" t="s">
-        <v>45</v>
-      </c>
       <c r="S19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T19" t="s">
         <v>26</v>
@@ -12023,10 +12020,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -12074,7 +12071,7 @@
         <v>30</v>
       </c>
       <c r="S20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T20" t="s">
         <v>24</v>
@@ -12095,13 +12092,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>43</v>
@@ -12140,13 +12137,13 @@
         <v>29</v>
       </c>
       <c r="Q21" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R21" t="s">
         <v>30</v>
       </c>
       <c r="S21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T21" t="s">
         <v>24</v>
@@ -12167,10 +12164,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
         <v>84</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -12239,16 +12236,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
@@ -12284,13 +12281,13 @@
         <v>40</v>
       </c>
       <c r="Q23" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R23" t="s">
         <v>30</v>
       </c>
       <c r="S23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T23" t="s">
         <v>26</v>
@@ -12311,10 +12308,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
         <v>88</v>
-      </c>
-      <c r="C24" t="s">
-        <v>89</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -12362,7 +12359,7 @@
         <v>30</v>
       </c>
       <c r="S24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T24" t="s">
         <v>26</v>
@@ -12383,13 +12380,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" t="s">
-        <v>91</v>
-      </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
@@ -12455,10 +12452,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
         <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -12500,13 +12497,13 @@
         <v>29</v>
       </c>
       <c r="Q26" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R26" t="s">
         <v>30</v>
       </c>
       <c r="S26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T26" t="s">
         <v>26</v>
@@ -12527,19 +12524,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
         <v>94</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
@@ -12572,13 +12569,13 @@
         <v>29</v>
       </c>
       <c r="Q27" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R27" t="s">
         <v>30</v>
       </c>
       <c r="S27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T27" t="s">
         <v>24</v>
@@ -12599,10 +12596,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -12644,13 +12641,13 @@
         <v>40</v>
       </c>
       <c r="Q28" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R28" t="s">
         <v>30</v>
       </c>
       <c r="S28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T28" t="s">
         <v>24</v>
@@ -12671,13 +12668,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
-      <c r="C29" t="s">
-        <v>99</v>
-      </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
@@ -12743,16 +12740,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
         <v>100</v>
       </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
         <v>24</v>
@@ -12788,13 +12785,13 @@
         <v>29</v>
       </c>
       <c r="Q30" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R30" t="s">
         <v>30</v>
       </c>
       <c r="S30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T30" t="s">
         <v>24</v>
@@ -12815,10 +12812,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
         <v>102</v>
-      </c>
-      <c r="C31" t="s">
-        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -12866,7 +12863,7 @@
         <v>30</v>
       </c>
       <c r="S31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T31" t="s">
         <v>26</v>
@@ -12887,19 +12884,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
         <v>104</v>
-      </c>
-      <c r="C32" t="s">
-        <v>105</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
         <v>37</v>
@@ -12932,13 +12929,13 @@
         <v>29</v>
       </c>
       <c r="Q32" t="s">
+        <v>60</v>
+      </c>
+      <c r="R32" t="s">
         <v>44</v>
       </c>
-      <c r="R32" t="s">
-        <v>45</v>
-      </c>
       <c r="S32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T32" t="s">
         <v>26</v>
@@ -12959,10 +12956,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
         <v>106</v>
-      </c>
-      <c r="C33" t="s">
-        <v>107</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -13007,10 +13004,10 @@
         <v>26</v>
       </c>
       <c r="R33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T33" t="s">
         <v>24</v>
@@ -13031,19 +13028,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
         <v>108</v>
       </c>
-      <c r="C34" t="s">
-        <v>109</v>
-      </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
         <v>37</v>
@@ -13076,13 +13073,13 @@
         <v>40</v>
       </c>
       <c r="Q34" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R34" t="s">
         <v>30</v>
       </c>
       <c r="S34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T34" t="s">
         <v>26</v>
@@ -13103,13 +13100,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
         <v>110</v>
       </c>
-      <c r="C35" t="s">
-        <v>111</v>
-      </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
         <v>34</v>
@@ -13154,7 +13151,7 @@
         <v>30</v>
       </c>
       <c r="S35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T35" t="s">
         <v>24</v>
@@ -13175,13 +13172,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
         <v>112</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>113</v>
-      </c>
-      <c r="D36" t="s">
-        <v>114</v>
       </c>
       <c r="E36" t="s">
         <v>34</v>
@@ -13226,7 +13223,7 @@
         <v>30</v>
       </c>
       <c r="S36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T36" t="s">
         <v>24</v>
@@ -13247,13 +13244,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
         <v>115</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>116</v>
-      </c>
-      <c r="D37" t="s">
-        <v>117</v>
       </c>
       <c r="E37" t="s">
         <v>34</v>
@@ -13319,10 +13316,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" t="s">
         <v>118</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
@@ -13370,7 +13367,7 @@
         <v>30</v>
       </c>
       <c r="S38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T38" t="s">
         <v>24</v>
@@ -13391,19 +13388,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>37</v>
@@ -13436,13 +13433,13 @@
         <v>40</v>
       </c>
       <c r="Q39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R39" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="S39" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T39" t="s">
         <v>26</v>
@@ -13463,13 +13460,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" t="s">
         <v>122</v>
       </c>
-      <c r="C40" t="s">
-        <v>123</v>
-      </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
@@ -13535,10 +13532,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
         <v>124</v>
-      </c>
-      <c r="C41" t="s">
-        <v>125</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -13607,10 +13604,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" t="s">
         <v>126</v>
-      </c>
-      <c r="C42" t="s">
-        <v>127</v>
       </c>
       <c r="D42" t="s">
         <v>22</v>
@@ -13619,7 +13616,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G42" t="s">
         <v>37</v>
@@ -13652,13 +13649,13 @@
         <v>29</v>
       </c>
       <c r="Q42" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R42" t="s">
         <v>30</v>
       </c>
       <c r="S42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T42" t="s">
         <v>24</v>
@@ -13679,10 +13676,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
         <v>128</v>
-      </c>
-      <c r="C43" t="s">
-        <v>129</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -13691,7 +13688,7 @@
         <v>34</v>
       </c>
       <c r="F43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G43" t="s">
         <v>25</v>
@@ -13730,7 +13727,7 @@
         <v>30</v>
       </c>
       <c r="S43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T43" t="s">
         <v>24</v>
@@ -13751,13 +13748,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" t="s">
         <v>130</v>
       </c>
-      <c r="C44" t="s">
-        <v>131</v>
-      </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" t="s">
         <v>34</v>
@@ -13823,10 +13820,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" t="s">
         <v>132</v>
-      </c>
-      <c r="C45" t="s">
-        <v>133</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -13895,10 +13892,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
         <v>134</v>
-      </c>
-      <c r="C46" t="s">
-        <v>135</v>
       </c>
       <c r="D46" t="s">
         <v>22</v>
@@ -13967,19 +13964,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>37</v>
@@ -14012,13 +14009,13 @@
         <v>40</v>
       </c>
       <c r="Q47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R47" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="S47" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T47" t="s">
         <v>26</v>
@@ -14039,19 +14036,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>37</v>
@@ -14084,13 +14081,13 @@
         <v>40</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>30</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T48" t="s">
         <v>26</v>
@@ -14111,10 +14108,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" t="s">
         <v>140</v>
-      </c>
-      <c r="C49" t="s">
-        <v>141</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -14162,7 +14159,7 @@
         <v>30</v>
       </c>
       <c r="S49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T49" t="s">
         <v>24</v>
@@ -14183,10 +14180,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" t="s">
         <v>142</v>
-      </c>
-      <c r="C50" t="s">
-        <v>143</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -14255,10 +14252,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -14300,13 +14297,13 @@
         <v>40</v>
       </c>
       <c r="Q51" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R51" t="s">
         <v>30</v>
       </c>
       <c r="S51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T51" t="s">
         <v>24</v>
@@ -14327,10 +14324,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" t="s">
         <v>145</v>
-      </c>
-      <c r="C52" t="s">
-        <v>146</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
@@ -14372,10 +14369,10 @@
         <v>29</v>
       </c>
       <c r="Q52" t="s">
+        <v>60</v>
+      </c>
+      <c r="R52" t="s">
         <v>44</v>
-      </c>
-      <c r="R52" t="s">
-        <v>45</v>
       </c>
       <c r="S52" t="s">
         <v>30</v>
@@ -14399,16 +14396,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" t="s">
         <v>147</v>
-      </c>
-      <c r="C53" t="s">
-        <v>148</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" t="s">
         <v>26</v>
@@ -14444,13 +14441,13 @@
         <v>29</v>
       </c>
       <c r="Q53" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R53" t="s">
         <v>30</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T53" t="s">
         <v>26</v>
@@ -14471,10 +14468,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" t="s">
         <v>149</v>
-      </c>
-      <c r="C54" t="s">
-        <v>150</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -14522,7 +14519,7 @@
         <v>30</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T54" t="s">
         <v>26</v>
@@ -14543,16 +14540,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" t="s">
         <v>151</v>
-      </c>
-      <c r="C55" t="s">
-        <v>152</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F55" t="s">
         <v>26</v>
@@ -14588,13 +14585,13 @@
         <v>29</v>
       </c>
       <c r="Q55" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R55" t="s">
         <v>30</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T55" t="s">
         <v>26</v>
@@ -14615,10 +14612,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>22</v>
@@ -14627,7 +14624,7 @@
         <v>43</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>37</v>
@@ -14660,13 +14657,13 @@
         <v>40</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R56" s="3" t="s">
         <v>30</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T56" t="s">
         <v>26</v>
@@ -14687,10 +14684,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" t="s">
         <v>155</v>
-      </c>
-      <c r="C57" t="s">
-        <v>156</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -14738,7 +14735,7 @@
         <v>30</v>
       </c>
       <c r="S57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T57" t="s">
         <v>24</v>
@@ -14759,10 +14756,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
         <v>157</v>
-      </c>
-      <c r="C58" t="s">
-        <v>158</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -14831,10 +14828,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" t="s">
         <v>159</v>
-      </c>
-      <c r="C59" t="s">
-        <v>160</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -14882,7 +14879,7 @@
         <v>30</v>
       </c>
       <c r="S59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T59" t="s">
         <v>24</v>
@@ -14903,19 +14900,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>37</v>
@@ -14948,13 +14945,13 @@
         <v>40</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R60" s="3" t="s">
         <v>30</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T60" t="s">
         <v>26</v>
@@ -14975,16 +14972,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" t="s">
         <v>163</v>
       </c>
-      <c r="C61" t="s">
-        <v>164</v>
-      </c>
       <c r="D61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" t="s">
         <v>24</v>
@@ -15020,13 +15017,13 @@
         <v>29</v>
       </c>
       <c r="Q61" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R61" t="s">
         <v>30</v>
       </c>
       <c r="S61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T61" t="s">
         <v>24</v>
@@ -15047,10 +15044,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" t="s">
         <v>165</v>
-      </c>
-      <c r="C62" t="s">
-        <v>166</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -15098,7 +15095,7 @@
         <v>30</v>
       </c>
       <c r="S62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T62" t="s">
         <v>24</v>
@@ -15119,19 +15116,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>37</v>
@@ -15164,13 +15161,13 @@
         <v>40</v>
       </c>
       <c r="Q63" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R63" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R63" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="S63" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T63" t="s">
         <v>26</v>
@@ -15191,13 +15188,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="s">
         <v>169</v>
       </c>
-      <c r="C64" t="s">
-        <v>170</v>
-      </c>
       <c r="D64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E64" t="s">
         <v>34</v>
@@ -15236,13 +15233,13 @@
         <v>29</v>
       </c>
       <c r="Q64" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="R64" t="s">
         <v>30</v>
       </c>
       <c r="S64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T64" t="s">
         <v>26</v>
@@ -15263,13 +15260,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" t="s">
         <v>171</v>
       </c>
-      <c r="C65" t="s">
-        <v>172</v>
-      </c>
       <c r="D65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E65" t="s">
         <v>34</v>
@@ -15335,10 +15332,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" t="s">
         <v>173</v>
-      </c>
-      <c r="C66" t="s">
-        <v>174</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -15407,13 +15404,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" t="s">
         <v>175</v>
       </c>
-      <c r="C67" t="s">
-        <v>176</v>
-      </c>
       <c r="D67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E67" t="s">
         <v>34</v>
@@ -15458,7 +15455,7 @@
         <v>30</v>
       </c>
       <c r="S67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T67" t="s">
         <v>24</v>
@@ -15479,10 +15476,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
         <v>177</v>
-      </c>
-      <c r="C68" t="s">
-        <v>178</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -15530,7 +15527,7 @@
         <v>30</v>
       </c>
       <c r="S68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T68" t="s">
         <v>26</v>
@@ -15551,10 +15548,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" t="s">
         <v>179</v>
-      </c>
-      <c r="C69" t="s">
-        <v>180</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -15602,7 +15599,7 @@
         <v>30</v>
       </c>
       <c r="S69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T69" t="s">
         <v>24</v>
@@ -15623,13 +15620,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
         <v>181</v>
       </c>
-      <c r="C70" t="s">
-        <v>182</v>
-      </c>
       <c r="D70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E70" t="s">
         <v>43</v>
@@ -15668,10 +15665,10 @@
         <v>29</v>
       </c>
       <c r="Q70" t="s">
+        <v>60</v>
+      </c>
+      <c r="R70" t="s">
         <v>44</v>
-      </c>
-      <c r="R70" t="s">
-        <v>45</v>
       </c>
       <c r="S70" t="s">
         <v>30</v>
@@ -15695,19 +15692,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>37</v>
@@ -15740,13 +15737,13 @@
         <v>40</v>
       </c>
       <c r="Q71" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R71" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R71" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="S71" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T71" t="s">
         <v>26</v>
@@ -15767,13 +15764,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" t="s">
         <v>185</v>
       </c>
-      <c r="C72" t="s">
-        <v>186</v>
-      </c>
       <c r="D72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E72" t="s">
         <v>34</v>
@@ -15818,7 +15815,7 @@
         <v>30</v>
       </c>
       <c r="S72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T72" t="s">
         <v>24</v>
@@ -15839,13 +15836,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" t="s">
         <v>187</v>
       </c>
-      <c r="C73" t="s">
-        <v>188</v>
-      </c>
       <c r="D73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E73" t="s">
         <v>34</v>
@@ -15890,7 +15887,7 @@
         <v>30</v>
       </c>
       <c r="S73" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T73" t="s">
         <v>24</v>

</xml_diff>